<commit_message>
Updated OpenGL status and matrix
</commit_message>
<xml_diff>
--- a/doc/OpenGL Drivers Status.xlsx
+++ b/doc/OpenGL Drivers Status.xlsx
@@ -36,6 +36,34 @@
     <author>Groove</author>
   </authors>
   <commentList>
+    <comment ref="C53" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Return 4.40 for the GLSL version</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C56" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>glGetNamedFramebufferAttachmentParameteriv generates an invalid enum error with GL_SAMPLES</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C57" authorId="0" shapeId="0">
       <text>
         <r>
@@ -10182,7 +10210,7 @@
                   <c:v>0.875</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.63636363636363635</c:v>
+                  <c:v>0.45454545454545453</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.90909090909090906</c:v>
@@ -10312,8 +10340,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1277406592"/>
-        <c:axId val="-1277402784"/>
+        <c:axId val="1492874784"/>
+        <c:axId val="1492875328"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -10459,7 +10487,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1277406592"/>
+        <c:axId val="1492874784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10469,7 +10497,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1277402784"/>
+        <c:crossAx val="1492875328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10477,7 +10505,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1277402784"/>
+        <c:axId val="1492875328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -10489,7 +10517,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1277406592"/>
+        <c:crossAx val="1492874784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10845,11 +10873,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1090101456"/>
-        <c:axId val="-1090111248"/>
+        <c:axId val="1662824032"/>
+        <c:axId val="1662822400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1090101456"/>
+        <c:axId val="1662824032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10859,7 +10887,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1090111248"/>
+        <c:crossAx val="1662822400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10867,7 +10895,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1090111248"/>
+        <c:axId val="1662822400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -10879,7 +10907,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1090101456"/>
+        <c:crossAx val="1662824032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11386,11 +11414,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1090112880"/>
-        <c:axId val="-1090110704"/>
+        <c:axId val="1662820224"/>
+        <c:axId val="1662820768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1090112880"/>
+        <c:axId val="1662820224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11400,7 +11428,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1090110704"/>
+        <c:crossAx val="1662820768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11408,7 +11436,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1090110704"/>
+        <c:axId val="1662820768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -11420,7 +11448,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1090112880"/>
+        <c:crossAx val="1662820224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11891,11 +11919,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1090109616"/>
-        <c:axId val="-1090104176"/>
+        <c:axId val="1662815328"/>
+        <c:axId val="1662821312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1090109616"/>
+        <c:axId val="1662815328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11905,7 +11933,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1090104176"/>
+        <c:crossAx val="1662821312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11913,7 +11941,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1090104176"/>
+        <c:axId val="1662821312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -11925,7 +11953,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1090109616"/>
+        <c:crossAx val="1662815328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12258,8 +12286,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1277406048"/>
-        <c:axId val="-1277402240"/>
+        <c:axId val="1660700240"/>
+        <c:axId val="1660705136"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -12405,7 +12433,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1277406048"/>
+        <c:axId val="1660700240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12415,7 +12443,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1277402240"/>
+        <c:crossAx val="1660705136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12423,7 +12451,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1277402240"/>
+        <c:axId val="1660705136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -12435,7 +12463,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1277406048"/>
+        <c:crossAx val="1660700240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12894,11 +12922,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1277401696"/>
-        <c:axId val="-1277414208"/>
+        <c:axId val="1660701328"/>
+        <c:axId val="1660694800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1277401696"/>
+        <c:axId val="1660701328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12908,7 +12936,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1277414208"/>
+        <c:crossAx val="1660694800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12916,7 +12944,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1277414208"/>
+        <c:axId val="1660694800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -12928,7 +12956,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1277401696"/>
+        <c:crossAx val="1660701328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13379,11 +13407,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1277413664"/>
-        <c:axId val="-1277408768"/>
+        <c:axId val="1660702416"/>
+        <c:axId val="1660707312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1277413664"/>
+        <c:axId val="1660702416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13393,7 +13421,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1277408768"/>
+        <c:crossAx val="1660707312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13401,7 +13429,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1277408768"/>
+        <c:axId val="1660707312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -13413,7 +13441,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1277413664"/>
+        <c:crossAx val="1660702416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13792,11 +13820,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1277404960"/>
-        <c:axId val="-1279201696"/>
+        <c:axId val="1660699696"/>
+        <c:axId val="1660700784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1277404960"/>
+        <c:axId val="1660699696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13806,7 +13834,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1279201696"/>
+        <c:crossAx val="1660700784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13814,7 +13842,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1279201696"/>
+        <c:axId val="1660700784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -13826,7 +13854,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1277404960"/>
+        <c:crossAx val="1660699696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14205,11 +14233,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1090105808"/>
-        <c:axId val="-1090109072"/>
+        <c:axId val="1660704048"/>
+        <c:axId val="1660696432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1090105808"/>
+        <c:axId val="1660704048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14219,7 +14247,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1090109072"/>
+        <c:crossAx val="1660696432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14227,7 +14255,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1090109072"/>
+        <c:axId val="1660696432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -14239,7 +14267,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1090105808"/>
+        <c:crossAx val="1660704048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14618,11 +14646,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1090113968"/>
-        <c:axId val="-1090103088"/>
+        <c:axId val="1660698064"/>
+        <c:axId val="1660698608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1090113968"/>
+        <c:axId val="1660698064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14632,7 +14660,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1090103088"/>
+        <c:crossAx val="1660698608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14640,7 +14668,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1090103088"/>
+        <c:axId val="1660698608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -14652,7 +14680,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1090113968"/>
+        <c:crossAx val="1660698064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15031,11 +15059,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1090107984"/>
-        <c:axId val="-1090099824"/>
+        <c:axId val="1660705680"/>
+        <c:axId val="1660692624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1090107984"/>
+        <c:axId val="1660705680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15045,7 +15073,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1090099824"/>
+        <c:crossAx val="1660692624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15053,7 +15081,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1090099824"/>
+        <c:axId val="1660692624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -15065,7 +15093,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1090107984"/>
+        <c:crossAx val="1660705680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15420,11 +15448,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1090102544"/>
-        <c:axId val="-1090106352"/>
+        <c:axId val="1662813696"/>
+        <c:axId val="1662822944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1090102544"/>
+        <c:axId val="1662813696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15434,7 +15462,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1090106352"/>
+        <c:crossAx val="1662822944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15442,7 +15470,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1090106352"/>
+        <c:axId val="1662822944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -15454,7 +15482,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1090102544"/>
+        <c:crossAx val="1662813696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16204,8 +16232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K348"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+    <sheetView tabSelected="1" topLeftCell="A277" workbookViewId="0">
+      <selection activeCell="C281" sqref="C281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16371,7 +16399,7 @@
       </c>
       <c r="C13" s="75">
         <f t="shared" ref="C13:D13" si="1">IF(C$66=0, 0,(C$61+C$62)/C$86)</f>
-        <v>0.63636363636363635</v>
+        <v>0.45454545454545453</v>
       </c>
       <c r="D13" s="75">
         <f t="shared" si="1"/>
@@ -16860,8 +16888,8 @@
       <c r="B53" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C53" s="4" t="s">
-        <v>6</v>
+      <c r="C53" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="D53" s="96" t="s">
         <v>175</v>
@@ -16902,8 +16930,8 @@
       <c r="B56" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C56" s="4" t="s">
-        <v>6</v>
+      <c r="C56" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="D56" s="96" t="s">
         <v>175</v>
@@ -16975,7 +17003,7 @@
       </c>
       <c r="C61" s="84">
         <f t="shared" ref="C61:D61" si="10">COUNTIF(C53:C60,"pass")</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D61" s="84">
         <f t="shared" si="10"/>
@@ -17026,7 +17054,7 @@
       </c>
       <c r="C64" s="86">
         <f t="shared" ref="C64:D64" si="13">COUNTIF(C53:C60,"Fail")</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D64" s="86">
         <f t="shared" si="13"/>

</xml_diff>